<commit_message>
Ejercicio final casi terminado
</commit_message>
<xml_diff>
--- a/27_02_2023/UL054239_proyect.xlsx
+++ b/27_02_2023/UL054239_proyect.xlsx
@@ -1,103 +1,100 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:workbookPr codeName="ThisWorkbook"/>
-  <x:bookViews>
-    <x:workbookView firstSheet="0" activeTab="0"/>
-  </x:bookViews>
-  <x:sheets>
-    <x:sheet name="Hoja1" sheetId="2" r:id="rId2"/>
-  </x:sheets>
-  <x:definedNames/>
-  <x:calcPr calcId="125725"/>
-</x:workbook>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://atentoglobal-my.sharepoint.com/personal/z28943283_es_atento_com/Documents/Documentos/Proyecto-Nuevo/27_02_2023/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_A1FC0FD2E10AA980847676AA465DEBDF2D290A38" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4C8657E-FD5C-402B-8D41-F23E2D9496EC}"/>
+  <bookViews>
+    <workbookView xWindow="735" yWindow="1575" windowWidth="20460" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Hoja1" sheetId="2" r:id="rId1"/>
+  </sheets>
+  <calcPr calcId="0"/>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <x:si>
-    <x:t>Project Name</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Type</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Code</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Description</x:t>
-  </x:si>
-  <x:si>
-    <x:t>UL054239</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Investigación</x:t>
-  </x:si>
-  <x:si>
-    <x:t>RES</x:t>
-  </x:si>
-  <x:si>
-    <x:t>un estudio de viabilidad o la investigación de un producto químico</x:t>
-  </x:si>
-</x:sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>Project Name</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>UL054239</t>
+  </si>
+  <si>
+    <t>Investigación</t>
+  </si>
+  <si>
+    <t>RES</t>
+  </si>
+  <si>
+    <t>un estudio de viabilidad o la investigación de un producto químico</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:numFmts count="1">
-    <x:numFmt numFmtId="0" formatCode=""/>
-  </x:numFmts>
-  <x:fonts count="1">
-    <x:font>
-      <x:vertAlign val="baseline"/>
-      <x:sz val="11"/>
-      <x:color rgb="FF000000"/>
-      <x:name val="Calibri"/>
-      <x:family val="2"/>
-    </x:font>
-  </x:fonts>
-  <x:fills count="2">
-    <x:fill>
-      <x:patternFill patternType="none"/>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="gray125"/>
-    </x:fill>
-  </x:fills>
-  <x:borders count="1">
-    <x:border diagonalUp="0" diagonalDown="0">
-      <x:left style="none">
-        <x:color rgb="FF000000"/>
-      </x:left>
-      <x:right style="none">
-        <x:color rgb="FF000000"/>
-      </x:right>
-      <x:top style="none">
-        <x:color rgb="FF000000"/>
-      </x:top>
-      <x:bottom style="none">
-        <x:color rgb="FF000000"/>
-      </x:bottom>
-      <x:diagonal style="none">
-        <x:color rgb="FF000000"/>
-      </x:diagonal>
-    </x:border>
-  </x:borders>
-  <x:cellStyleXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-  </x:cellStyleXfs>
-  <x:cellXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-  </x:cellXfs>
-  <x:cellStyles count="1">
-    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </x:cellStyles>
-</x:styleSheet>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+  </fonts>
+  <fills count="2">
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
+  </fills>
+  <borders count="1">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+  </borders>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
+  </cellStyleXfs>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+  </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
+</styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -384,49 +381,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:sheetPr>
-    <x:outlinePr summaryBelow="1" summaryRight="1"/>
-  </x:sheetPr>
-  <x:dimension ref="A1:D2"/>
-  <x:sheetViews>
-    <x:sheetView workbookViewId="0"/>
-  </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15"/>
-  <x:sheetData>
-    <x:row r="1" spans="1:4">
-      <x:c r="A1" s="0" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="B1" s="0" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C1" s="0" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="D1" s="0" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:4">
-      <x:c r="A2" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="B2" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="C2" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="D2" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-    </x:row>
-  </x:sheetData>
-  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
-  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
-  <x:headerFooter/>
-  <x:tableParts count="0"/>
-</x:worksheet>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+</worksheet>
 </file>
</xml_diff>